<commit_message>
added respiration subplots to sampling locations
</commit_message>
<xml_diff>
--- a/Setup/Sampling_locations.xlsx
+++ b/Setup/Sampling_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Research/NutNet/Setup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/NutNet_LBK/Setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3EA1774-8C5F-2248-9D56-01F51ACC1105}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19C59F-6CB0-C542-91A0-4F9C70372A1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{25DD38BB-498C-6145-AA2D-555984D5204E}"/>
+    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="14220" xr2:uid="{25DD38BB-498C-6145-AA2D-555984D5204E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="20">
   <si>
     <t>Plot</t>
   </si>
@@ -46,6 +46,45 @@
   </si>
   <si>
     <t>SW</t>
+  </si>
+  <si>
+    <t>Subplot_respiration</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>xControl</t>
+  </si>
+  <si>
+    <t>NPK+Fence</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>NPK</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>Fence</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -397,489 +436,711 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BC1B78-0EBC-B44C-A21D-B6BE106CAAAB}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised sampling locations due to Nick's error on soil collar placement
</commit_message>
<xml_diff>
--- a/Setup/Sampling_locations.xlsx
+++ b/Setup/Sampling_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/NutNet_LBK/Setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19C59F-6CB0-C542-91A0-4F9C70372A1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998BD833-1D38-F142-9ECF-FFE4FD6478D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="14220" xr2:uid="{25DD38BB-498C-6145-AA2D-555984D5204E}"/>
   </bookViews>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BC1B78-0EBC-B44C-A21D-B6BE106CAAAB}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1024,7 +1024,7 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
slight update to sampling locations
</commit_message>
<xml_diff>
--- a/Setup/Sampling_locations.xlsx
+++ b/Setup/Sampling_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicksmith/Documents/Git/NutNet_LBK/Setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157EAA54-A9E1-FB4A-B9A2-253979CB7ED2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365212BA-B9DC-1248-AB29-D6DC712853AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="2200" windowWidth="28040" windowHeight="15880" xr2:uid="{25DD38BB-498C-6145-AA2D-555984D5204E}"/>
+    <workbookView xWindow="9420" yWindow="2200" windowWidth="28040" windowHeight="15880" xr2:uid="{25DD38BB-498C-6145-AA2D-555984D5204E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,17 +450,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BC1B78-0EBC-B44C-A21D-B6BE106CAAAB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1430,6 +1433,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="76" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="8"/>
 </worksheet>
 </file>
</xml_diff>